<commit_message>
Started 2nd topic - expanded use cases
</commit_message>
<xml_diff>
--- a/Expanded Use Cases.xlsx
+++ b/Expanded Use Cases.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCE33F0-1D8F-4D77-9F56-201ED5EF5B58}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7656" windowHeight="2304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
   <si>
     <t>Use Case</t>
   </si>
@@ -61,59 +62,139 @@
   </si>
   <si>
     <t>System Response</t>
-  </si>
-  <si>
-    <t>1. The use case begins with the user
-adding a new member</t>
-  </si>
-  <si>
-    <t>2. The user enters the member details</t>
-  </si>
-  <si>
-    <t>3. Checks the database if the member exists</t>
-  </si>
-  <si>
-    <t>4. Pops up an error message if the member
- already exists. Otherwise, pops up a successful message</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user decides to add a new member to the
-Café. The user obtains the member details such as his/her name, date of birth, home address, contact number, e-mail address and membership type. The system will check the database to see if the member already exists and pop up an error message, if the member already exists. Otherwise, a successful message will pop up when the process is complete. The user can return to the home page. </t>
-  </si>
-  <si>
-    <t>5. The user returns to the home page</t>
-  </si>
-  <si>
-    <t>2. The user enters the details obtained from
- the customer</t>
-  </si>
-  <si>
-    <t>3. Checks if the customer is a member or not</t>
-  </si>
-  <si>
-    <t>4. Displays the session timings and price based on
-the member status</t>
-  </si>
-  <si>
-    <t>5. The user selects the requested session
- duration</t>
-  </si>
-  <si>
-    <t>6. A successful message will pop up when the
-booking is complete</t>
-  </si>
-  <si>
-    <t>7. The user can return to the home page</t>
-  </si>
-  <si>
-    <t>1. This use case begins with the user making
-a booking for a customer</t>
   </si>
   <si>
     <t xml:space="preserve">The user decides to book a game for the customer.
 The user obtains the details from the customer
 such as date and time, the platform, classic/chart and
 Singe Player/Multiplayer. The cost of the sessions  will be calculated by the system if the customer is a member or not and will be displayed to the user. The user will  then select the requested session duration. A successful message will appear when the booking is successful. The user can return to the home page. </t>
+  </si>
+  <si>
+    <t>Book for an Event</t>
+  </si>
+  <si>
+    <t>Book for an ESport Event in the Game Café</t>
+  </si>
+  <si>
+    <t>The user decides to book an event for the customer.
+The user will only proceed with the process if the customer is a member of the café. If the customer is a member, the user will obtain the details needed for the booking such as number of tickets and data and time of the event. The user will then enter the payment details. A successful message will pop up when the booking is successful. The user can return to the home page.</t>
+  </si>
+  <si>
+    <t>5. The system will make an contact with the bank
+and verify the transaction.</t>
+  </si>
+  <si>
+    <t>1. This use case begins with the user
+making an event booking for a customer.</t>
+  </si>
+  <si>
+    <t>2. The user confirms if the customer is
+a member.</t>
+  </si>
+  <si>
+    <t>3. If yes, the user will enter the event
+details required for booking.</t>
+  </si>
+  <si>
+    <t>4. The user will enter the payment
+ details (for card payment).</t>
+  </si>
+  <si>
+    <t>1. The use case begins with the user
+adding a new member.</t>
+  </si>
+  <si>
+    <t>2. The user enters the member details.</t>
+  </si>
+  <si>
+    <t>1. This use case begins with the user making
+a game booking for a customer.</t>
+  </si>
+  <si>
+    <t>2. The user enters the details obtained from
+ the customer.</t>
+  </si>
+  <si>
+    <t>5. The user selects the requested session
+ duration.</t>
+  </si>
+  <si>
+    <t>7. The user can return to the home page.</t>
+  </si>
+  <si>
+    <t>6. A successful message will pop up when the
+booking is complete.</t>
+  </si>
+  <si>
+    <t>4. Displays the session timings and price based on
+the member status.</t>
+  </si>
+  <si>
+    <t>3. Checks if the customer is a member or not.</t>
+  </si>
+  <si>
+    <t>7. The user can return to the home
+page.</t>
+  </si>
+  <si>
+    <t>6. A successful message will be displayed if the
+booking process is successful.</t>
+  </si>
+  <si>
+    <t>View Member Information</t>
+  </si>
+  <si>
+    <t>To view member information and details</t>
+  </si>
+  <si>
+    <t>Secondary</t>
+  </si>
+  <si>
+    <t>1. This use case begins with
+the user viewing member
+information</t>
+  </si>
+  <si>
+    <t>2. The sytem displays the list of members in the café.</t>
+  </si>
+  <si>
+    <t>3. The user selects a
+member.</t>
+  </si>
+  <si>
+    <t>5. The user can return to the home page.</t>
+  </si>
+  <si>
+    <t>4. The system displays information on the chosen
+member.</t>
+  </si>
+  <si>
+    <t>The user decides to view member details and
+information on any bookings done under his/her name. The system will display the list of members in the cafe. The user will then select a member he/she wishes to view. The system will then display the chosen member's contact details, membership type, how long has he/she been a member in the café, etc. The user can return to home page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user decides to add a new member to the
+Café. The user obtains the member details such as his/her name, date of birth, home address, contact number, e-mail address and membership type. The age of the member must be 18 or above years. The system will pop an error if the user entered a lower age. It will also pop an error if the e-mail address is invalid. The system will check the database to see if the member already exists and pop up an error message, if the member already exists. Otherwise, a successful message will pop up when the process is complete. The user can return to the home page. </t>
+  </si>
+  <si>
+    <t>3. Checks if the age entered is 18 or above</t>
+  </si>
+  <si>
+    <t>4. Pops up an error message if the age is below</t>
+  </si>
+  <si>
+    <t>5. Check if the entered e-mail address is valid.</t>
+  </si>
+  <si>
+    <t>6. Pops up an error message if the address is invalid</t>
+  </si>
+  <si>
+    <t>7. A successful message will pop when the
+registration is complete.</t>
+  </si>
+  <si>
+    <t>8. The user can return to the home
+ page.</t>
   </si>
 </sst>
 </file>
@@ -220,13 +301,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -512,24 +593,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:H16"/>
+  <dimension ref="C3:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="32.21875" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" style="2" customWidth="1"/>
     <col min="7" max="7" width="38.109375" customWidth="1"/>
     <col min="8" max="8" width="41.5546875" customWidth="1"/>
     <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="11" max="11" width="31.6640625" customWidth="1"/>
+    <col min="12" max="12" width="43" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" customWidth="1"/>
+    <col min="16" max="16" width="44.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:16" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
@@ -542,8 +627,20 @@
       <c r="H3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
@@ -556,8 +653,20 @@
       <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="3:8" ht="48.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" ht="48.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
@@ -570,22 +679,46 @@
       <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" ht="189" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" ht="215.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -598,84 +731,179 @@
       <c r="H7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="3:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="6" t="s">
+      <c r="K7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="3:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="G9" s="6" t="s">
+      <c r="D9" s="8"/>
+      <c r="G9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="3:8" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="8" t="s">
+      <c r="H9" s="8"/>
+      <c r="K9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="O9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" spans="3:16" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C12" s="5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="O12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L13" s="2"/>
+      <c r="O13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="5" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="O14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="3:16" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="6"/>
+      <c r="D15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="3:8" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="L15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="3:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D16" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="3:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="3:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C18" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="G9:H9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="O9:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Started Topic 4 - AE1
</commit_message>
<xml_diff>
--- a/Expanded Use Cases.xlsx
+++ b/Expanded Use Cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCE33F0-1D8F-4D77-9F56-201ED5EF5B58}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E2BEE0-A8D0-40D3-9577-2DB11B7C8C56}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7656" windowHeight="2304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,21 +180,23 @@
     <t>3. Checks if the age entered is 18 or above</t>
   </si>
   <si>
-    <t>4. Pops up an error message if the age is below</t>
-  </si>
-  <si>
-    <t>5. Check if the entered e-mail address is valid.</t>
-  </si>
-  <si>
-    <t>6. Pops up an error message if the address is invalid</t>
-  </si>
-  <si>
-    <t>7. A successful message will pop when the
+    <t>5. A successful message will pop when the
 registration is complete.</t>
   </si>
   <si>
-    <t>8. The user can return to the home
+    <t>6. The user can return to the home
  page.</t>
+  </si>
+  <si>
+    <t>4. Check if the entered e-mail address is valid.</t>
+  </si>
+  <si>
+    <t>Alternate Flow of Events</t>
+  </si>
+  <si>
+    <t>Line 3. Invalid age entered. Indicate
+Error. Return to Step 2.
+Invalid e-mail address entered. Indicate error. Return to Step 2.</t>
   </si>
 </sst>
 </file>
@@ -284,7 +286,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -309,6 +311,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -593,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:P18"/>
+  <dimension ref="C3:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,8 +838,8 @@
       </c>
     </row>
     <row r="14" spans="3:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="5" t="s">
-        <v>45</v>
+      <c r="D14" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="5" t="s">
@@ -851,8 +856,8 @@
     </row>
     <row r="15" spans="3:16" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="6"/>
-      <c r="D15" s="2" t="s">
-        <v>46</v>
+      <c r="D15" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>27</v>
@@ -870,9 +875,10 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="3:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D16" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="C16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="G16" t="s">
         <v>28</v>
       </c>
@@ -884,26 +890,31 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="3:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D17" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="K17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="3:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C18" s="5" t="s">
+    <row r="18" spans="3:16" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="3:16" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="3:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C20" s="4" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="O9:P9"/>
+    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>